<commit_message>
Test Data updates - 10 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyBothPrimaryAndNonPrimaryAttendeeCanEditFollowUpActivity.xlsx
+++ b/TestData/TMTC0032668_VerifyBothPrimaryAndNonPrimaryAttendeeCanEditFollowUpActivity.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C05AB1C-1EE8-4C3C-A974-7C2D5A4E3850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949FAD8F-739E-43F7-95BD-A4C156DFFDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
     <sheet name="Followup" sheetId="12" r:id="rId4"/>
+    <sheet name="MoreAttendees" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Users</t>
   </si>
@@ -126,6 +127,15 @@
   </si>
   <si>
     <t>Internal Followup</t>
+  </si>
+  <si>
+    <t>HLAttendee</t>
+  </si>
+  <si>
+    <t>Test James</t>
+  </si>
+  <si>
+    <t>Amanda Donovan</t>
   </si>
 </sst>
 </file>
@@ -629,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -662,4 +672,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7A37C3-BB8A-428A-AFE4-550098595333}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
10 Sep 2024 - Final
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyBothPrimaryAndNonPrimaryAttendeeCanEditFollowUpActivity.xlsx
+++ b/TestData/TMTC0032668_VerifyBothPrimaryAndNonPrimaryAttendeeCanEditFollowUpActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949FAD8F-739E-43F7-95BD-A4C156DFFDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25DF86D-CE31-4E43-AE5C-C51FF75D8262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
     <sheet name="Followup" sheetId="12" r:id="rId4"/>
     <sheet name="MoreAttendees" sheetId="13" r:id="rId5"/>
+    <sheet name="UpdateActivity" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Users</t>
   </si>
@@ -136,6 +137,27 @@
   </si>
   <si>
     <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>Updated Primary Attendee</t>
+  </si>
+  <si>
+    <t>FIG - Financial Institutions</t>
+  </si>
+  <si>
+    <t>Advisory</t>
+  </si>
+  <si>
+    <t>Updated Test Description Primary Attendee</t>
+  </si>
+  <si>
+    <t>Updated Notes</t>
+  </si>
+  <si>
+    <t>Updated Non Primary Attendee</t>
+  </si>
+  <si>
+    <t>Updated Test Description Non Primary Attendee</t>
   </si>
 </sst>
 </file>
@@ -678,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7A37C3-BB8A-428A-AFE4-550098595333}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -707,4 +729,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D89725F-8DE6-44A6-93E3-1301DACA2D5D}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>